<commit_message>
changed names in boxplot
</commit_message>
<xml_diff>
--- a/Validation project/Data and Script/Data/selected genes for validation.xlsx
+++ b/Validation project/Data and Script/Data/selected genes for validation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha.gcupadhaya\Desktop\RNA-seq\Validation project\Data and Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha.gcupadhaya\Desktop\RNA-seq\Validation project\Data and Script\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0707F8A-E771-4293-B755-E3BDE3251E8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071B2953-9078-4E50-AEBD-2C45C76A4DCE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="4" xr2:uid="{76CDB992-AAAC-4221-A4D3-B456CA4663FA}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{76CDB992-AAAC-4221-A4D3-B456CA4663FA}"/>
   </bookViews>
   <sheets>
     <sheet name="verticillium" sheetId="1" r:id="rId1"/>
@@ -8331,7 +8331,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8673,13 +8673,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178E5026-FA1C-4A56-8842-51F692E7AE81}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
@@ -10449,16 +10449,16 @@
       </c>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" t="s">
+      <c r="A63" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="9">
         <v>653</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="9">
         <v>4.8</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -10481,16 +10481,16 @@
       </c>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" t="s">
+      <c r="A64" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="9">
         <v>111</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="9">
         <v>-3.6</v>
       </c>
       <c r="E64" s="5" t="s">
@@ -10510,39 +10510,37 @@
       </c>
     </row>
     <row r="65" spans="1:10" s="33" customFormat="1">
-      <c r="A65" s="33" t="s">
+      <c r="A65" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="33">
+      <c r="B65" s="9">
         <v>111</v>
       </c>
-      <c r="C65" s="33" t="s">
+      <c r="C65" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="D65" s="9"/>
       <c r="E65" s="33" t="s">
         <v>27</v>
       </c>
       <c r="F65" s="35" t="s">
         <v>362</v>
       </c>
-      <c r="H65" s="33" t="s">
-        <v>29</v>
-      </c>
       <c r="I65" s="33" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" t="s">
+      <c r="A66" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="9">
         <v>111</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="9">
         <v>-4.7</v>
       </c>
       <c r="E66" t="s">
@@ -10551,8 +10549,8 @@
       <c r="G66" t="s">
         <v>28</v>
       </c>
-      <c r="H66" t="s">
-        <v>34</v>
+      <c r="H66" s="33" t="s">
+        <v>29</v>
       </c>
       <c r="I66" t="s">
         <v>338</v>
@@ -10610,7 +10608,7 @@
         <v>33</v>
       </c>
       <c r="H68" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I68" t="s">
         <v>338</v>
@@ -10688,7 +10686,7 @@
         <v>40</v>
       </c>
       <c r="H71" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="I71" t="s">
         <v>338</v>
@@ -10740,7 +10738,7 @@
         <v>42</v>
       </c>
       <c r="H73" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I73" t="s">
         <v>338</v>
@@ -10766,7 +10764,7 @@
         <v>46</v>
       </c>
       <c r="H74" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I74" t="s">
         <v>338</v>
@@ -10792,7 +10790,7 @@
         <v>50</v>
       </c>
       <c r="H75" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I75" t="s">
         <v>338</v>
@@ -10818,7 +10816,7 @@
         <v>54</v>
       </c>
       <c r="H76" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I76" t="s">
         <v>338</v>
@@ -10847,7 +10845,7 @@
         <v>58</v>
       </c>
       <c r="H77" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I77" t="s">
         <v>338</v>
@@ -10876,7 +10874,7 @@
         <v>64</v>
       </c>
       <c r="H78" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="I78" t="s">
         <v>338</v>
@@ -10928,7 +10926,7 @@
         <v>70</v>
       </c>
       <c r="H80" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="I80" t="s">
         <v>338</v>
@@ -10954,7 +10952,7 @@
         <v>72</v>
       </c>
       <c r="H81" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I81" t="s">
         <v>338</v>
@@ -10980,7 +10978,7 @@
         <v>75</v>
       </c>
       <c r="H82" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I82" t="s">
         <v>338</v>
@@ -11006,7 +11004,7 @@
         <v>79</v>
       </c>
       <c r="H83" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I83" t="s">
         <v>338</v>
@@ -11025,14 +11023,14 @@
       <c r="D84">
         <v>-2.8</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="26" t="s">
         <v>82</v>
       </c>
       <c r="G84" t="s">
         <v>83</v>
       </c>
       <c r="H84" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I84" t="s">
         <v>338</v>
@@ -11058,7 +11056,7 @@
         <v>87</v>
       </c>
       <c r="H85" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="I85" t="s">
         <v>338</v>
@@ -11084,7 +11082,7 @@
         <v>90</v>
       </c>
       <c r="H86" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="I86" t="s">
         <v>338</v>
@@ -11110,7 +11108,7 @@
         <v>93</v>
       </c>
       <c r="H87" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I87" t="s">
         <v>370</v>
@@ -11129,14 +11127,14 @@
       <c r="D88">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="5" t="s">
         <v>96</v>
       </c>
       <c r="G88" s="41" t="s">
         <v>97</v>
       </c>
       <c r="H88" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I88" t="s">
         <v>338</v>
@@ -11162,7 +11160,7 @@
         <v>101</v>
       </c>
       <c r="H89" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="I89" t="s">
         <v>338</v>
@@ -11186,6 +11184,9 @@
       </c>
       <c r="G90" t="s">
         <v>42</v>
+      </c>
+      <c r="H90" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:11">

</xml_diff>